<commit_message>
Chapter 3 part A done
</commit_message>
<xml_diff>
--- a/excel notes/Nand2Tetris2.xlsx
+++ b/excel notes/Nand2Tetris2.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="107">
   <si>
     <t>zx</t>
   </si>
@@ -298,12 +298,63 @@
   <si>
     <t xml:space="preserve"> 45+  </t>
   </si>
+  <si>
+    <t>reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> inc </t>
+  </si>
+  <si>
+    <t>load</t>
+  </si>
+  <si>
+    <t>inc</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>out(t-1)</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>out(t-1)+1</t>
+  </si>
+  <si>
+    <t>out=0</t>
+  </si>
+  <si>
+    <t>out(t)=in(t-1)</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>8-way 16 bit mux</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,8 +362,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,6 +393,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -457,13 +522,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,15 +553,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>218514</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>10086</xdr:rowOff>
+      <xdr:colOff>319367</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>54909</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>98349</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>9634</xdr:rowOff>
+      <xdr:colOff>199202</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>54457</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -517,7 +584,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11469220" y="4010586"/>
+          <a:off x="11570073" y="4436409"/>
           <a:ext cx="6536129" cy="3619048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -529,16 +596,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>496421</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>77320</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>104215</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>122144</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>400345</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>153296</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>8139</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -561,7 +628,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11142009" y="2363320"/>
+          <a:off x="11354921" y="2598644"/>
           <a:ext cx="6560218" cy="1790476"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -573,16 +640,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>327773</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>88526</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>294156</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>122144</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>160806</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>71278</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>127188</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>104896</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -605,7 +672,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13393832" y="4089026"/>
+          <a:off x="12755097" y="884144"/>
           <a:ext cx="4068856" cy="1316252"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -617,16 +684,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>138953</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>165846</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>463924</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>177052</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>337437</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>41819</xdr:rowOff>
+      <xdr:colOff>57290</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>53025</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -649,8 +716,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13205012" y="5880846"/>
+          <a:off x="12924865" y="7797052"/>
           <a:ext cx="3829190" cy="1209473"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>470647</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>134470</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>76992</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>47898</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E19F19BE-08B6-4A28-A3EE-5E44463DD2DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22613471" y="2991970"/>
+          <a:ext cx="7114286" cy="6771428"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1106,13 +1217,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R173"/>
+  <dimension ref="A1:AT173"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J43" sqref="J43"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AQ8" sqref="AQ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,9 +1230,10 @@
     <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -1167,8 +1276,26 @@
       <c r="R1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1216,8 +1343,26 @@
         <f>R1+1</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1273,8 +1418,29 @@
         <f t="shared" ref="R3:R66" si="2">R2+1</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH3" s="23">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="23">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="23">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="23">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="23">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="23">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1330,8 +1496,26 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH4" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI4" s="23">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="23">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="23">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="23">
+        <v>1</v>
+      </c>
+      <c r="AM4" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1387,8 +1571,38 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH5">
+        <v>2</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>1</v>
+      </c>
+      <c r="AM5">
+        <v>1</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -1444,8 +1658,41 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH6" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI6">
+        <v>-32123</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>1</v>
+      </c>
+      <c r="AM6">
+        <v>1</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <v>0</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1501,8 +1748,41 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH7" s="23">
+        <v>3</v>
+      </c>
+      <c r="AI7" s="23">
+        <v>-32123</v>
+      </c>
+      <c r="AJ7" s="23">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="23">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="23">
+        <v>1</v>
+      </c>
+      <c r="AM7" s="23">
+        <v>2</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>95</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>0</v>
+      </c>
+      <c r="AS7">
+        <v>1</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -1558,8 +1838,41 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH8" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI8" s="23">
+        <v>-32123</v>
+      </c>
+      <c r="AJ8" s="23">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="23">
+        <v>1</v>
+      </c>
+      <c r="AL8" s="23">
+        <v>1</v>
+      </c>
+      <c r="AM8" s="23">
+        <v>2</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
+      <c r="AR8">
+        <v>1</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1579,7 +1892,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="20">
         <v>1111</v>
       </c>
       <c r="I9">
@@ -1614,8 +1927,41 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH9">
+        <v>4</v>
+      </c>
+      <c r="AI9">
+        <v>-32123</v>
+      </c>
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <v>1</v>
+      </c>
+      <c r="AL9">
+        <v>1</v>
+      </c>
+      <c r="AM9">
+        <v>-32123</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ9">
+        <v>0</v>
+      </c>
+      <c r="AR9">
+        <v>1</v>
+      </c>
+      <c r="AS9">
+        <v>1</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1671,8 +2017,41 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH10" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI10">
+        <v>-32123</v>
+      </c>
+      <c r="AJ10">
+        <v>0</v>
+      </c>
+      <c r="AK10">
+        <v>0</v>
+      </c>
+      <c r="AL10">
+        <v>1</v>
+      </c>
+      <c r="AM10">
+        <v>-32123</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>103</v>
+      </c>
+      <c r="AQ10">
+        <v>1</v>
+      </c>
+      <c r="AR10">
+        <v>0</v>
+      </c>
+      <c r="AS10">
+        <v>0</v>
+      </c>
+      <c r="AT10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1728,8 +2107,41 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH11" s="23">
+        <v>5</v>
+      </c>
+      <c r="AI11" s="23">
+        <v>-32123</v>
+      </c>
+      <c r="AJ11" s="23">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="23">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="23">
+        <v>1</v>
+      </c>
+      <c r="AM11" s="23">
+        <v>-32122</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ11">
+        <v>1</v>
+      </c>
+      <c r="AR11">
+        <v>0</v>
+      </c>
+      <c r="AS11">
+        <v>1</v>
+      </c>
+      <c r="AT11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -1785,8 +2197,41 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH12" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI12" s="23">
+        <v>-32123</v>
+      </c>
+      <c r="AJ12" s="23">
+        <v>0</v>
+      </c>
+      <c r="AK12" s="23">
+        <v>0</v>
+      </c>
+      <c r="AL12" s="23">
+        <v>1</v>
+      </c>
+      <c r="AM12" s="23">
+        <v>-32122</v>
+      </c>
+      <c r="AP12" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ12">
+        <v>1</v>
+      </c>
+      <c r="AR12">
+        <v>1</v>
+      </c>
+      <c r="AS12">
+        <v>0</v>
+      </c>
+      <c r="AT12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1842,8 +2287,41 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH13">
+        <v>6</v>
+      </c>
+      <c r="AI13">
+        <v>-32123</v>
+      </c>
+      <c r="AJ13">
+        <v>0</v>
+      </c>
+      <c r="AK13">
+        <v>0</v>
+      </c>
+      <c r="AL13">
+        <v>1</v>
+      </c>
+      <c r="AM13">
+        <v>-32121</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>105</v>
+      </c>
+      <c r="AQ13">
+        <v>1</v>
+      </c>
+      <c r="AR13">
+        <v>1</v>
+      </c>
+      <c r="AS13">
+        <v>1</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -1899,8 +2377,26 @@
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH14" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI14">
+        <v>12345</v>
+      </c>
+      <c r="AJ14">
+        <v>0</v>
+      </c>
+      <c r="AK14">
+        <v>1</v>
+      </c>
+      <c r="AL14">
+        <v>0</v>
+      </c>
+      <c r="AM14">
+        <v>-32121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1928,7 +2424,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J15" s="22">
+      <c r="J15" s="20">
         <v>3333</v>
       </c>
       <c r="K15">
@@ -1955,8 +2451,26 @@
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH15" s="23">
+        <v>7</v>
+      </c>
+      <c r="AI15" s="23">
+        <v>12345</v>
+      </c>
+      <c r="AJ15" s="23">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="23">
+        <v>1</v>
+      </c>
+      <c r="AL15" s="23">
+        <v>0</v>
+      </c>
+      <c r="AM15" s="23">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -2012,8 +2526,26 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH16" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI16" s="23">
+        <v>12345</v>
+      </c>
+      <c r="AJ16" s="23">
+        <v>1</v>
+      </c>
+      <c r="AK16" s="23">
+        <v>1</v>
+      </c>
+      <c r="AL16" s="23">
+        <v>0</v>
+      </c>
+      <c r="AM16" s="23">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>8</v>
       </c>
@@ -2069,8 +2601,26 @@
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH17">
+        <v>8</v>
+      </c>
+      <c r="AI17">
+        <v>12345</v>
+      </c>
+      <c r="AJ17">
+        <v>1</v>
+      </c>
+      <c r="AK17">
+        <v>1</v>
+      </c>
+      <c r="AL17">
+        <v>0</v>
+      </c>
+      <c r="AM17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>8</v>
       </c>
@@ -2126,8 +2676,26 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH18" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI18">
+        <v>12345</v>
+      </c>
+      <c r="AJ18">
+        <v>0</v>
+      </c>
+      <c r="AK18">
+        <v>1</v>
+      </c>
+      <c r="AL18">
+        <v>1</v>
+      </c>
+      <c r="AM18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -2183,8 +2751,27 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH19" s="23">
+        <v>9</v>
+      </c>
+      <c r="AI19" s="23">
+        <v>12345</v>
+      </c>
+      <c r="AJ19" s="23">
+        <v>0</v>
+      </c>
+      <c r="AK19" s="23">
+        <v>1</v>
+      </c>
+      <c r="AL19" s="23">
+        <v>1</v>
+      </c>
+      <c r="AM19" s="23">
+        <v>12345</v>
+      </c>
+      <c r="AP19" s="2"/>
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>9</v>
       </c>
@@ -2240,8 +2827,26 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH20" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI20" s="23">
+        <v>12345</v>
+      </c>
+      <c r="AJ20" s="23">
+        <v>1</v>
+      </c>
+      <c r="AK20" s="23">
+        <v>1</v>
+      </c>
+      <c r="AL20" s="23">
+        <v>1</v>
+      </c>
+      <c r="AM20" s="23">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -2297,8 +2902,26 @@
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH21">
+        <v>10</v>
+      </c>
+      <c r="AI21">
+        <v>12345</v>
+      </c>
+      <c r="AJ21">
+        <v>1</v>
+      </c>
+      <c r="AK21">
+        <v>1</v>
+      </c>
+      <c r="AL21">
+        <v>1</v>
+      </c>
+      <c r="AM21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10</v>
       </c>
@@ -2342,7 +2965,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="N22" s="22">
+      <c r="N22" s="20">
         <v>7777</v>
       </c>
       <c r="P22">
@@ -2353,8 +2976,26 @@
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI22">
+        <v>12345</v>
+      </c>
+      <c r="AJ22">
+        <v>0</v>
+      </c>
+      <c r="AK22">
+        <v>0</v>
+      </c>
+      <c r="AL22">
+        <v>1</v>
+      </c>
+      <c r="AM22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2410,8 +3051,26 @@
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH23" s="23">
+        <v>11</v>
+      </c>
+      <c r="AI23" s="23">
+        <v>12345</v>
+      </c>
+      <c r="AJ23" s="23">
+        <v>0</v>
+      </c>
+      <c r="AK23" s="23">
+        <v>0</v>
+      </c>
+      <c r="AL23" s="23">
+        <v>1</v>
+      </c>
+      <c r="AM23" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>11</v>
       </c>
@@ -2467,8 +3126,26 @@
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH24" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI24" s="23">
+        <v>12345</v>
+      </c>
+      <c r="AJ24" s="23">
+        <v>1</v>
+      </c>
+      <c r="AK24" s="23">
+        <v>0</v>
+      </c>
+      <c r="AL24" s="23">
+        <v>1</v>
+      </c>
+      <c r="AM24" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>11</v>
       </c>
@@ -2524,8 +3201,26 @@
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH25">
+        <v>12</v>
+      </c>
+      <c r="AI25">
+        <v>12345</v>
+      </c>
+      <c r="AJ25">
+        <v>1</v>
+      </c>
+      <c r="AK25">
+        <v>0</v>
+      </c>
+      <c r="AL25">
+        <v>1</v>
+      </c>
+      <c r="AM25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>11</v>
       </c>
@@ -2581,8 +3276,26 @@
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH26" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI26">
+        <v>0</v>
+      </c>
+      <c r="AJ26">
+        <v>0</v>
+      </c>
+      <c r="AK26">
+        <v>1</v>
+      </c>
+      <c r="AL26">
+        <v>1</v>
+      </c>
+      <c r="AM26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -2638,8 +3351,26 @@
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH27">
+        <v>13</v>
+      </c>
+      <c r="AI27">
+        <v>0</v>
+      </c>
+      <c r="AJ27">
+        <v>0</v>
+      </c>
+      <c r="AK27">
+        <v>1</v>
+      </c>
+      <c r="AL27">
+        <v>1</v>
+      </c>
+      <c r="AM27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>12</v>
       </c>
@@ -2695,8 +3426,26 @@
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH28" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI28" s="23">
+        <v>0</v>
+      </c>
+      <c r="AJ28" s="23">
+        <v>0</v>
+      </c>
+      <c r="AK28" s="23">
+        <v>0</v>
+      </c>
+      <c r="AL28" s="23">
+        <v>1</v>
+      </c>
+      <c r="AM28" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>12</v>
       </c>
@@ -2752,8 +3501,26 @@
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH29" s="23">
+        <v>14</v>
+      </c>
+      <c r="AI29" s="23">
+        <v>0</v>
+      </c>
+      <c r="AJ29" s="23">
+        <v>0</v>
+      </c>
+      <c r="AK29" s="23">
+        <v>0</v>
+      </c>
+      <c r="AL29" s="23">
+        <v>1</v>
+      </c>
+      <c r="AM29" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>12</v>
       </c>
@@ -2809,8 +3576,26 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH30" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI30">
+        <v>22222</v>
+      </c>
+      <c r="AJ30">
+        <v>1</v>
+      </c>
+      <c r="AK30">
+        <v>0</v>
+      </c>
+      <c r="AL30">
+        <v>0</v>
+      </c>
+      <c r="AM30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>12</v>
       </c>
@@ -2866,8 +3651,26 @@
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AH31">
+        <v>15</v>
+      </c>
+      <c r="AI31">
+        <v>22222</v>
+      </c>
+      <c r="AJ31">
+        <v>1</v>
+      </c>
+      <c r="AK31">
+        <v>0</v>
+      </c>
+      <c r="AL31">
+        <v>0</v>
+      </c>
+      <c r="AM31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>12</v>
       </c>
@@ -3168,7 +3971,7 @@
       <c r="E37">
         <v>21845</v>
       </c>
-      <c r="G37" s="22">
+      <c r="G37" s="20">
         <v>21845</v>
       </c>
       <c r="H37">
@@ -3285,7 +4088,7 @@
         <f t="shared" si="3"/>
         <v>21845</v>
       </c>
-      <c r="H39" s="22">
+      <c r="H39" s="20">
         <v>21845</v>
       </c>
       <c r="I39">
@@ -3402,7 +4205,7 @@
         <f t="shared" si="4"/>
         <v>21845</v>
       </c>
-      <c r="I41" s="22">
+      <c r="I41" s="20">
         <v>21845</v>
       </c>
       <c r="J41">
@@ -3519,7 +4322,7 @@
         <f t="shared" si="5"/>
         <v>21845</v>
       </c>
-      <c r="J43" s="22">
+      <c r="J43" s="20">
         <v>21845</v>
       </c>
       <c r="K43">
@@ -10959,7 +11762,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -15068,30 +15872,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="L1" s="20" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="L1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
       <c r="V1" s="15"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -53911,40 +54715,40 @@
       <c r="N2" s="17"/>
     </row>
     <row r="3" spans="10:24" x14ac:dyDescent="0.25">
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
       <c r="Q3" s="19"/>
-      <c r="R3" s="21" t="s">
+      <c r="R3" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="21"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="22"/>
     </row>
     <row r="4" spans="10:24" x14ac:dyDescent="0.25">
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
       <c r="Q4" s="19"/>
-      <c r="R4" s="21" t="s">
+      <c r="R4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="S4" s="21"/>
-      <c r="T4" s="21"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="21"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
     </row>
     <row r="5" spans="10:24" x14ac:dyDescent="0.25">
       <c r="K5" s="7" t="s">

</xml_diff>